<commit_message>
list ur space edit done
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1533,39 +1533,79 @@
           <t>Pranjal Shukla</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
+      <c r="F28" t="n">
+        <v>9935558059</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>propques</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>pranjalshukla800@gmail.com</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>67bf00d01950ca48d9b97686</t>
+        </is>
+      </c>
+      <c r="J28" t="n">
+        <v>26.9107501</v>
+      </c>
+      <c r="K28" t="n">
+        <v>80.9465604</v>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Aliganj, Lucknow, Uttar Pradesh, 226024, India</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Pranjal Shukla</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
         <is>
           <t>9935558059</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>propques</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>pranjalshukla800@gmail.com</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>67bf00d01950ca48d9b97686</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>26.9107501</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>80.9465604</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>Aliganj, Lucknow, Uttar Pradesh, 226024, India</t>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>propques</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>pranjalshukla800@gmail.com</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>67c15dea7a5466fe052ba655</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>26.9176756</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>80.9539367</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>LU New Campus Road, Aliganj, Lucknow, Uttar Pradesh, 226026, India</t>
         </is>
       </c>
     </row>

</xml_diff>